<commit_message>
1. Implementing new parameters for outlier downweigthing on ears algorithm and all related application parameters 2. Fixing bug making topics dissapear after a while
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/topics.xlsx
+++ b/epitweetr/inst/extdata/topics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="161">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outliers Alpha</t>
   </si>
   <si>
     <t xml:space="preserve">Query</t>
@@ -776,27 +779,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="139.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="139.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,10 +816,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -824,32 +828,38 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">LEN(E2)</f>
+      <c r="E2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">LEN(F2)</f>
         <v>66</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <f aca="false">LEN(TRIM(E2))-LEN(SUBSTITUTE(E2," ",""))+1</f>
+      <c r="H2" s="0" t="n">
+        <f aca="false">LEN(TRIM(F2))-LEN(SUBSTITUTE(F2," ",""))+1</f>
         <v>11</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -858,26 +868,29 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <f aca="false">LEN(E3)</f>
+      <c r="E3" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">LEN(F3)</f>
         <v>51</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">LEN(TRIM(E3))-LEN(SUBSTITUTE(E3," ",""))+1</f>
+      <c r="H3" s="0" t="n">
+        <f aca="false">LEN(TRIM(F3))-LEN(SUBSTITUTE(F3," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -886,26 +899,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">LEN(F4)</f>
+        <v>78</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">LEN(TRIM(F4))-LEN(SUBSTITUTE(F4," ",""))+1</f>
         <v>13</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <f aca="false">LEN(E4)</f>
-        <v>78</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">LEN(TRIM(E4))-LEN(SUBSTITUTE(E4," ",""))+1</f>
-        <v>13</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -914,26 +930,29 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <f aca="false">LEN(E5)</f>
+      <c r="E5" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">LEN(F5)</f>
         <v>59</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">LEN(TRIM(E5))-LEN(SUBSTITUTE(E5," ",""))+1</f>
+      <c r="H5" s="0" t="n">
+        <f aca="false">LEN(TRIM(F5))-LEN(SUBSTITUTE(F5," ",""))+1</f>
         <v>13</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -942,26 +961,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <f aca="false">LEN(E6)</f>
+      <c r="E6" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">LEN(F6)</f>
         <v>129</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">LEN(TRIM(E6))-LEN(SUBSTITUTE(E6," ",""))+1</f>
+      <c r="H6" s="0" t="n">
+        <f aca="false">LEN(TRIM(F6))-LEN(SUBSTITUTE(F6," ",""))+1</f>
         <v>18</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -970,26 +992,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <f aca="false">LEN(E7)</f>
+      <c r="E7" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">LEN(F7)</f>
         <v>113</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">LEN(TRIM(E7))-LEN(SUBSTITUTE(E7," ",""))+1</f>
+      <c r="H7" s="0" t="n">
+        <f aca="false">LEN(TRIM(F7))-LEN(SUBSTITUTE(F7," ",""))+1</f>
         <v>22</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -998,26 +1023,29 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <f aca="false">LEN(E8)</f>
+      <c r="E8" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">LEN(F8)</f>
         <v>70</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">LEN(TRIM(E8))-LEN(SUBSTITUTE(E8," ",""))+1</f>
+      <c r="H8" s="0" t="n">
+        <f aca="false">LEN(TRIM(F8))-LEN(SUBSTITUTE(F8," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1026,26 +1054,29 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <f aca="false">LEN(E9)</f>
+      <c r="E9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">LEN(F9)</f>
         <v>95</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">LEN(TRIM(E9))-LEN(SUBSTITUTE(E9," ",""))+1</f>
+      <c r="H9" s="0" t="n">
+        <f aca="false">LEN(TRIM(F9))-LEN(SUBSTITUTE(F9," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1054,26 +1085,29 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <f aca="false">LEN(E10)</f>
+      <c r="E10" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">LEN(F10)</f>
         <v>42</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">LEN(TRIM(E10))-LEN(SUBSTITUTE(E10," ",""))+1</f>
+      <c r="H10" s="0" t="n">
+        <f aca="false">LEN(TRIM(F10))-LEN(SUBSTITUTE(F10," ",""))+1</f>
         <v>5</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1082,26 +1116,29 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <f aca="false">LEN(E11)</f>
+      <c r="E11" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">LEN(F11)</f>
         <v>134</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">LEN(TRIM(E11))-LEN(SUBSTITUTE(E11," ",""))+1</f>
+      <c r="H11" s="0" t="n">
+        <f aca="false">LEN(TRIM(F11))-LEN(SUBSTITUTE(F11," ",""))+1</f>
         <v>18</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1110,26 +1147,29 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">LEN(F12)</f>
+        <v>173</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">LEN(TRIM(F12))-LEN(SUBSTITUTE(F12," ",""))+1</f>
         <v>28</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <f aca="false">LEN(E12)</f>
-        <v>173</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">LEN(TRIM(E12))-LEN(SUBSTITUTE(E12," ",""))+1</f>
-        <v>28</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1138,26 +1178,29 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <f aca="false">LEN(E13)</f>
+      <c r="E13" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">LEN(F13)</f>
         <v>150</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">LEN(TRIM(E13))-LEN(SUBSTITUTE(E13," ",""))+1</f>
+      <c r="H13" s="0" t="n">
+        <f aca="false">LEN(TRIM(F13))-LEN(SUBSTITUTE(F13," ",""))+1</f>
         <v>24</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1166,26 +1209,29 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <f aca="false">LEN(E14)</f>
+      <c r="E14" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">LEN(F14)</f>
         <v>236</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">LEN(TRIM(E14))-LEN(SUBSTITUTE(E14," ",""))+1</f>
+      <c r="H14" s="0" t="n">
+        <f aca="false">LEN(TRIM(F14))-LEN(SUBSTITUTE(F14," ",""))+1</f>
         <v>36</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="I14" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1194,26 +1240,29 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <f aca="false">LEN(E15)</f>
+      <c r="E15" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">LEN(F15)</f>
         <v>255</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">LEN(TRIM(E15))-LEN(SUBSTITUTE(E15," ",""))+1</f>
+      <c r="H15" s="0" t="n">
+        <f aca="false">LEN(TRIM(F15))-LEN(SUBSTITUTE(F15," ",""))+1</f>
         <v>28</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="I15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1222,26 +1271,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <f aca="false">LEN(E16)</f>
+      <c r="E16" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">LEN(F16)</f>
         <v>187</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">LEN(TRIM(E16))-LEN(SUBSTITUTE(E16," ",""))+1</f>
+      <c r="H16" s="0" t="n">
+        <f aca="false">LEN(TRIM(F16))-LEN(SUBSTITUTE(F16," ",""))+1</f>
         <v>20</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="I16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1250,26 +1302,29 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <f aca="false">LEN(E17)</f>
+      <c r="E17" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">LEN(F17)</f>
         <v>52</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">LEN(TRIM(E17))-LEN(SUBSTITUTE(E17," ",""))+1</f>
+      <c r="H17" s="0" t="n">
+        <f aca="false">LEN(TRIM(F17))-LEN(SUBSTITUTE(F17," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1278,26 +1333,29 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <f aca="false">LEN(E18)</f>
+      <c r="E18" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">LEN(F18)</f>
         <v>177</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">LEN(TRIM(E18))-LEN(SUBSTITUTE(E18," ",""))+1</f>
+      <c r="H18" s="0" t="n">
+        <f aca="false">LEN(TRIM(F18))-LEN(SUBSTITUTE(F18," ",""))+1</f>
         <v>28</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1306,26 +1364,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <f aca="false">LEN(E19)</f>
+      <c r="E19" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">LEN(F19)</f>
         <v>193</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">LEN(TRIM(E19))-LEN(SUBSTITUTE(E19," ",""))+1</f>
+      <c r="H19" s="0" t="n">
+        <f aca="false">LEN(TRIM(F19))-LEN(SUBSTITUTE(F19," ",""))+1</f>
         <v>27</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1334,26 +1395,29 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <f aca="false">LEN(E20)</f>
+      <c r="E20" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">LEN(F20)</f>
         <v>209</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">LEN(TRIM(E20))-LEN(SUBSTITUTE(E20," ",""))+1</f>
+      <c r="H20" s="0" t="n">
+        <f aca="false">LEN(TRIM(F20))-LEN(SUBSTITUTE(F20," ",""))+1</f>
         <v>30</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1362,26 +1426,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <f aca="false">LEN(E21)</f>
+      <c r="E21" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">LEN(F21)</f>
         <v>52</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">LEN(TRIM(E21))-LEN(SUBSTITUTE(E21," ",""))+1</f>
+      <c r="H21" s="0" t="n">
+        <f aca="false">LEN(TRIM(F21))-LEN(SUBSTITUTE(F21," ",""))+1</f>
         <v>8</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1390,26 +1457,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <f aca="false">LEN(E22)</f>
+      <c r="E22" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">LEN(F22)</f>
         <v>158</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">LEN(TRIM(E22))-LEN(SUBSTITUTE(E22," ",""))+1</f>
+      <c r="H22" s="0" t="n">
+        <f aca="false">LEN(TRIM(F22))-LEN(SUBSTITUTE(F22," ",""))+1</f>
         <v>20</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="I22" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1418,26 +1488,29 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <f aca="false">LEN(E23)</f>
+      <c r="E23" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">LEN(F23)</f>
         <v>72</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">LEN(TRIM(E23))-LEN(SUBSTITUTE(E23," ",""))+1</f>
+      <c r="H23" s="0" t="n">
+        <f aca="false">LEN(TRIM(F23))-LEN(SUBSTITUTE(F23," ",""))+1</f>
         <v>11</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1446,26 +1519,29 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <f aca="false">LEN(E24)</f>
+      <c r="E24" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">LEN(F24)</f>
         <v>97</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">LEN(TRIM(E24))-LEN(SUBSTITUTE(E24," ",""))+1</f>
+      <c r="H24" s="0" t="n">
+        <f aca="false">LEN(TRIM(F24))-LEN(SUBSTITUTE(F24," ",""))+1</f>
         <v>12</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="I24" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1474,26 +1550,29 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <f aca="false">LEN(E25)</f>
+      <c r="E25" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">LEN(F25)</f>
         <v>60</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">LEN(TRIM(E25))-LEN(SUBSTITUTE(E25," ",""))+1</f>
+      <c r="H25" s="0" t="n">
+        <f aca="false">LEN(TRIM(F25))-LEN(SUBSTITUTE(F25," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1502,26 +1581,29 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <f aca="false">LEN(E26)</f>
+      <c r="E26" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">LEN(F26)</f>
         <v>210</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">LEN(TRIM(E26))-LEN(SUBSTITUTE(E26," ",""))+1</f>
+      <c r="H26" s="0" t="n">
+        <f aca="false">LEN(TRIM(F26))-LEN(SUBSTITUTE(F26," ",""))+1</f>
         <v>32</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1530,26 +1612,29 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <f aca="false">LEN(E27)</f>
+      <c r="E27" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">LEN(F27)</f>
         <v>93</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">LEN(TRIM(E27))-LEN(SUBSTITUTE(E27," ",""))+1</f>
+      <c r="H27" s="0" t="n">
+        <f aca="false">LEN(TRIM(F27))-LEN(SUBSTITUTE(F27," ",""))+1</f>
         <v>14</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="I27" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1558,26 +1643,29 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <f aca="false">LEN(E28)</f>
+      <c r="E28" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">LEN(F28)</f>
         <v>118</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">LEN(TRIM(E28))-LEN(SUBSTITUTE(E28," ",""))+1</f>
+      <c r="H28" s="0" t="n">
+        <f aca="false">LEN(TRIM(F28))-LEN(SUBSTITUTE(F28," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="I28" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1586,26 +1674,29 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <f aca="false">LEN(E29)</f>
+      <c r="E29" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">LEN(F29)</f>
         <v>193</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">LEN(TRIM(E29))-LEN(SUBSTITUTE(E29," ",""))+1</f>
+      <c r="H29" s="0" t="n">
+        <f aca="false">LEN(TRIM(F29))-LEN(SUBSTITUTE(F29," ",""))+1</f>
         <v>18</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="I29" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1614,26 +1705,29 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <f aca="false">LEN(E30)</f>
+      <c r="E30" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">LEN(F30)</f>
         <v>150</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">LEN(TRIM(E30))-LEN(SUBSTITUTE(E30," ",""))+1</f>
+      <c r="H30" s="0" t="n">
+        <f aca="false">LEN(TRIM(F30))-LEN(SUBSTITUTE(F30," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="I30" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1642,26 +1736,29 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <f aca="false">LEN(E31)</f>
+      <c r="E31" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">LEN(F31)</f>
         <v>69</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">LEN(TRIM(E31))-LEN(SUBSTITUTE(E31," ",""))+1</f>
+      <c r="H31" s="0" t="n">
+        <f aca="false">LEN(TRIM(F31))-LEN(SUBSTITUTE(F31," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="I31" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1670,26 +1767,29 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <f aca="false">LEN(E32)</f>
+      <c r="E32" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">LEN(F32)</f>
         <v>100</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">LEN(TRIM(E32))-LEN(SUBSTITUTE(E32," ",""))+1</f>
+      <c r="H32" s="0" t="n">
+        <f aca="false">LEN(TRIM(F32))-LEN(SUBSTITUTE(F32," ",""))+1</f>
         <v>12</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="I32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1698,26 +1798,29 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <f aca="false">LEN(E33)</f>
+      <c r="E33" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">LEN(F33)</f>
         <v>155</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">LEN(TRIM(E33))-LEN(SUBSTITUTE(E33," ",""))+1</f>
+      <c r="H33" s="0" t="n">
+        <f aca="false">LEN(TRIM(F33))-LEN(SUBSTITUTE(F33," ",""))+1</f>
         <v>20</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="I33" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1726,26 +1829,29 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <f aca="false">LEN(E34)</f>
+      <c r="E34" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">LEN(F34)</f>
         <v>97</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <f aca="false">LEN(TRIM(E34))-LEN(SUBSTITUTE(E34," ",""))+1</f>
+      <c r="H34" s="0" t="n">
+        <f aca="false">LEN(TRIM(F34))-LEN(SUBSTITUTE(F34," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="I34" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1754,26 +1860,29 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <f aca="false">LEN(E35)</f>
+      <c r="E35" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f aca="false">LEN(F35)</f>
         <v>80</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <f aca="false">LEN(TRIM(E35))-LEN(SUBSTITUTE(E35," ",""))+1</f>
+      <c r="H35" s="0" t="n">
+        <f aca="false">LEN(TRIM(F35))-LEN(SUBSTITUTE(F35," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1782,26 +1891,29 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <f aca="false">LEN(E36)</f>
+      <c r="E36" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f aca="false">LEN(F36)</f>
         <v>61</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">LEN(TRIM(E36))-LEN(SUBSTITUTE(E36," ",""))+1</f>
+      <c r="H36" s="0" t="n">
+        <f aca="false">LEN(TRIM(F36))-LEN(SUBSTITUTE(F36," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="I36" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1810,26 +1922,29 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <f aca="false">LEN(E37)</f>
+      <c r="E37" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">LEN(F37)</f>
         <v>155</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">LEN(TRIM(E37))-LEN(SUBSTITUTE(E37," ",""))+1</f>
+      <c r="H37" s="0" t="n">
+        <f aca="false">LEN(TRIM(F37))-LEN(SUBSTITUTE(F37," ",""))+1</f>
         <v>19</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="I37" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1838,26 +1953,29 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <f aca="false">LEN(E38)</f>
+      <c r="E38" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">LEN(F38)</f>
         <v>24</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <f aca="false">LEN(TRIM(E38))-LEN(SUBSTITUTE(E38," ",""))+1</f>
+      <c r="H38" s="0" t="n">
+        <f aca="false">LEN(TRIM(F38))-LEN(SUBSTITUTE(F38," ",""))+1</f>
         <v>2</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="I38" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1866,26 +1984,29 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <f aca="false">LEN(E39)</f>
+      <c r="E39" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">LEN(F39)</f>
         <v>10</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <f aca="false">LEN(TRIM(E39))-LEN(SUBSTITUTE(E39," ",""))+1</f>
-        <v>1</v>
-      </c>
       <c r="H39" s="0" t="n">
+        <f aca="false">LEN(TRIM(F39))-LEN(SUBSTITUTE(F39," ",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="I39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1894,26 +2015,29 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <f aca="false">LEN(E40)</f>
+      <c r="E40" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">LEN(F40)</f>
         <v>50</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <f aca="false">LEN(TRIM(E40))-LEN(SUBSTITUTE(E40," ",""))+1</f>
+      <c r="H40" s="0" t="n">
+        <f aca="false">LEN(TRIM(F40))-LEN(SUBSTITUTE(F40," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="I40" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1922,26 +2046,29 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <f aca="false">LEN(E41)</f>
+      <c r="E41" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">LEN(F41)</f>
         <v>90</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <f aca="false">LEN(TRIM(E41))-LEN(SUBSTITUTE(E41," ",""))+1</f>
+      <c r="H41" s="0" t="n">
+        <f aca="false">LEN(TRIM(F41))-LEN(SUBSTITUTE(F41," ",""))+1</f>
         <v>19</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="I41" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1950,26 +2077,29 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <f aca="false">LEN(E42)</f>
+      <c r="E42" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">LEN(F42)</f>
         <v>76</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <f aca="false">LEN(TRIM(E42))-LEN(SUBSTITUTE(E42," ",""))+1</f>
+      <c r="H42" s="0" t="n">
+        <f aca="false">LEN(TRIM(F42))-LEN(SUBSTITUTE(F42," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="I42" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1978,26 +2108,29 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <f aca="false">LEN(E43)</f>
+      <c r="E43" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">LEN(F43)</f>
         <v>181</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <f aca="false">LEN(TRIM(E43))-LEN(SUBSTITUTE(E43," ",""))+1</f>
+      <c r="H43" s="0" t="n">
+        <f aca="false">LEN(TRIM(F43))-LEN(SUBSTITUTE(F43," ",""))+1</f>
         <v>25</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="I43" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2006,26 +2139,29 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <f aca="false">LEN(E44)</f>
+      <c r="E44" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">LEN(F44)</f>
         <v>158</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <f aca="false">LEN(TRIM(E44))-LEN(SUBSTITUTE(E44," ",""))+1</f>
+      <c r="H44" s="0" t="n">
+        <f aca="false">LEN(TRIM(F44))-LEN(SUBSTITUTE(F44," ",""))+1</f>
         <v>18</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="I44" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2034,26 +2170,29 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <f aca="false">LEN(E45)</f>
+      <c r="E45" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">LEN(F45)</f>
         <v>172</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <f aca="false">LEN(TRIM(E45))-LEN(SUBSTITUTE(E45," ",""))+1</f>
+      <c r="H45" s="0" t="n">
+        <f aca="false">LEN(TRIM(F45))-LEN(SUBSTITUTE(F45," ",""))+1</f>
         <v>27</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="I45" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2062,26 +2201,29 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <f aca="false">LEN(E46)</f>
+      <c r="E46" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f aca="false">LEN(F46)</f>
         <v>75</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <f aca="false">LEN(TRIM(E46))-LEN(SUBSTITUTE(E46," ",""))+1</f>
+      <c r="H46" s="0" t="n">
+        <f aca="false">LEN(TRIM(F46))-LEN(SUBSTITUTE(F46," ",""))+1</f>
         <v>14</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="I46" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2090,26 +2232,29 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <f aca="false">LEN(E47)</f>
+      <c r="E47" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f aca="false">LEN(F47)</f>
         <v>190</v>
       </c>
-      <c r="G47" s="0" t="n">
-        <f aca="false">LEN(TRIM(E47))-LEN(SUBSTITUTE(E47," ",""))+1</f>
+      <c r="H47" s="0" t="n">
+        <f aca="false">LEN(TRIM(F47))-LEN(SUBSTITUTE(F47," ",""))+1</f>
         <v>24</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="I47" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2118,26 +2263,29 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <f aca="false">LEN(E48)</f>
+      <c r="E48" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <f aca="false">LEN(F48)</f>
         <v>118</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <f aca="false">LEN(TRIM(E48))-LEN(SUBSTITUTE(E48," ",""))+1</f>
+      <c r="H48" s="0" t="n">
+        <f aca="false">LEN(TRIM(F48))-LEN(SUBSTITUTE(F48," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="I48" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2146,26 +2294,29 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <f aca="false">LEN(E49)</f>
+      <c r="E49" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <f aca="false">LEN(F49)</f>
         <v>66</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <f aca="false">LEN(TRIM(E49))-LEN(SUBSTITUTE(E49," ",""))+1</f>
+      <c r="H49" s="0" t="n">
+        <f aca="false">LEN(TRIM(F49))-LEN(SUBSTITUTE(F49," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="I49" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2174,26 +2325,29 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <f aca="false">LEN(E50)</f>
+      <c r="E50" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">LEN(F50)</f>
         <v>139</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <f aca="false">LEN(TRIM(E50))-LEN(SUBSTITUTE(E50," ",""))+1</f>
+      <c r="H50" s="0" t="n">
+        <f aca="false">LEN(TRIM(F50))-LEN(SUBSTITUTE(F50," ",""))+1</f>
         <v>14</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="I50" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2202,26 +2356,29 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="0" t="n">
-        <f aca="false">LEN(E51)</f>
+      <c r="E51" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <f aca="false">LEN(F51)</f>
         <v>58</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <f aca="false">LEN(TRIM(E51))-LEN(SUBSTITUTE(E51," ",""))+1</f>
+      <c r="H51" s="0" t="n">
+        <f aca="false">LEN(TRIM(F51))-LEN(SUBSTITUTE(F51," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="I51" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2230,26 +2387,29 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <f aca="false">LEN(E52)</f>
+      <c r="E52" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <f aca="false">LEN(F52)</f>
         <v>207</v>
       </c>
-      <c r="G52" s="0" t="n">
-        <f aca="false">LEN(TRIM(E52))-LEN(SUBSTITUTE(E52," ",""))+1</f>
+      <c r="H52" s="0" t="n">
+        <f aca="false">LEN(TRIM(F52))-LEN(SUBSTITUTE(F52," ",""))+1</f>
         <v>24</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="I52" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2258,26 +2418,29 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <f aca="false">LEN(E53)</f>
+      <c r="E53" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <f aca="false">LEN(F53)</f>
         <v>73</v>
       </c>
-      <c r="G53" s="0" t="n">
-        <f aca="false">LEN(TRIM(E53))-LEN(SUBSTITUTE(E53," ",""))+1</f>
+      <c r="H53" s="0" t="n">
+        <f aca="false">LEN(TRIM(F53))-LEN(SUBSTITUTE(F53," ",""))+1</f>
         <v>14</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="I53" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2286,26 +2449,29 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <f aca="false">LEN(E54)</f>
+      <c r="E54" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <f aca="false">LEN(F54)</f>
         <v>168</v>
       </c>
-      <c r="G54" s="0" t="n">
-        <f aca="false">LEN(TRIM(E54))-LEN(SUBSTITUTE(E54," ",""))+1</f>
+      <c r="H54" s="0" t="n">
+        <f aca="false">LEN(TRIM(F54))-LEN(SUBSTITUTE(F54," ",""))+1</f>
         <v>34</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="I54" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2314,26 +2480,29 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <f aca="false">LEN(E55)</f>
+      <c r="E55" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <f aca="false">LEN(F55)</f>
         <v>74</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <f aca="false">LEN(TRIM(E55))-LEN(SUBSTITUTE(E55," ",""))+1</f>
+      <c r="H55" s="0" t="n">
+        <f aca="false">LEN(TRIM(F55))-LEN(SUBSTITUTE(F55," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="I55" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2342,26 +2511,29 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <f aca="false">LEN(E56)</f>
+      <c r="E56" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">LEN(F56)</f>
         <v>100</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <f aca="false">LEN(TRIM(E56))-LEN(SUBSTITUTE(E56," ",""))+1</f>
+      <c r="H56" s="0" t="n">
+        <f aca="false">LEN(TRIM(F56))-LEN(SUBSTITUTE(F56," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="I56" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2370,26 +2542,29 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">LEN(F57)</f>
         <v>114</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <f aca="false">LEN(E57)</f>
-        <v>114</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <f aca="false">LEN(TRIM(E57))-LEN(SUBSTITUTE(E57," ",""))+1</f>
+      <c r="H57" s="0" t="n">
+        <f aca="false">LEN(TRIM(F57))-LEN(SUBSTITUTE(F57," ",""))+1</f>
         <v>17</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="I57" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2398,26 +2573,29 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F58" s="0" t="n">
-        <f aca="false">LEN(E58)</f>
+      <c r="E58" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <f aca="false">LEN(F58)</f>
         <v>138</v>
       </c>
-      <c r="G58" s="0" t="n">
-        <f aca="false">LEN(TRIM(E58))-LEN(SUBSTITUTE(E58," ",""))+1</f>
+      <c r="H58" s="0" t="n">
+        <f aca="false">LEN(TRIM(F58))-LEN(SUBSTITUTE(F58," ",""))+1</f>
         <v>15</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="I58" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2426,26 +2604,29 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <f aca="false">LEN(E59)</f>
+      <c r="E59" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <f aca="false">LEN(F59)</f>
         <v>213</v>
       </c>
-      <c r="G59" s="0" t="n">
-        <f aca="false">LEN(TRIM(E59))-LEN(SUBSTITUTE(E59," ",""))+1</f>
+      <c r="H59" s="0" t="n">
+        <f aca="false">LEN(TRIM(F59))-LEN(SUBSTITUTE(F59," ",""))+1</f>
         <v>27</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="I59" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2454,26 +2635,29 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F60" s="0" t="n">
-        <f aca="false">LEN(E60)</f>
+      <c r="E60" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <f aca="false">LEN(F60)</f>
         <v>87</v>
       </c>
-      <c r="G60" s="0" t="n">
-        <f aca="false">LEN(TRIM(E60))-LEN(SUBSTITUTE(E60," ",""))+1</f>
+      <c r="H60" s="0" t="n">
+        <f aca="false">LEN(TRIM(F60))-LEN(SUBSTITUTE(F60," ",""))+1</f>
         <v>10</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="I60" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2482,26 +2666,29 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F61" s="0" t="n">
-        <f aca="false">LEN(E61)</f>
+      <c r="E61" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <f aca="false">LEN(F61)</f>
         <v>167</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <f aca="false">LEN(TRIM(E61))-LEN(SUBSTITUTE(E61," ",""))+1</f>
+      <c r="H61" s="0" t="n">
+        <f aca="false">LEN(TRIM(F61))-LEN(SUBSTITUTE(F61," ",""))+1</f>
         <v>21</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="I61" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2510,26 +2697,29 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <f aca="false">LEN(E62)</f>
+      <c r="E62" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <f aca="false">LEN(F62)</f>
         <v>246</v>
       </c>
-      <c r="G62" s="0" t="n">
-        <f aca="false">LEN(TRIM(E62))-LEN(SUBSTITUTE(E62," ",""))+1</f>
+      <c r="H62" s="0" t="n">
+        <f aca="false">LEN(TRIM(F62))-LEN(SUBSTITUTE(F62," ",""))+1</f>
         <v>33</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="I62" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2538,26 +2728,29 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F63" s="0" t="n">
-        <f aca="false">LEN(E63)</f>
+      <c r="E63" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <f aca="false">LEN(F63)</f>
         <v>72</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <f aca="false">LEN(TRIM(E63))-LEN(SUBSTITUTE(E63," ",""))+1</f>
+      <c r="H63" s="0" t="n">
+        <f aca="false">LEN(TRIM(F63))-LEN(SUBSTITUTE(F63," ",""))+1</f>
         <v>11</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="I63" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2566,26 +2759,29 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <f aca="false">LEN(E64)</f>
+      <c r="E64" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <f aca="false">LEN(F64)</f>
         <v>37</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <f aca="false">LEN(TRIM(E64))-LEN(SUBSTITUTE(E64," ",""))+1</f>
+      <c r="H64" s="0" t="n">
+        <f aca="false">LEN(TRIM(F64))-LEN(SUBSTITUTE(F64," ",""))+1</f>
         <v>5</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="I64" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2594,26 +2790,29 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <f aca="false">LEN(E65)</f>
+      <c r="E65" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <f aca="false">LEN(F65)</f>
         <v>119</v>
       </c>
-      <c r="G65" s="0" t="n">
-        <f aca="false">LEN(TRIM(E65))-LEN(SUBSTITUTE(E65," ",""))+1</f>
+      <c r="H65" s="0" t="n">
+        <f aca="false">LEN(TRIM(F65))-LEN(SUBSTITUTE(F65," ",""))+1</f>
         <v>20</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="I65" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2622,26 +2821,29 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <f aca="false">LEN(E66)</f>
+      <c r="E66" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <f aca="false">LEN(F66)</f>
         <v>46</v>
       </c>
-      <c r="G66" s="0" t="n">
-        <f aca="false">LEN(TRIM(E66))-LEN(SUBSTITUTE(E66," ",""))+1</f>
+      <c r="H66" s="0" t="n">
+        <f aca="false">LEN(TRIM(F66))-LEN(SUBSTITUTE(F66," ",""))+1</f>
         <v>5</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="I66" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2650,26 +2852,29 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <f aca="false">LEN(E67)</f>
+      <c r="E67" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <f aca="false">LEN(F67)</f>
         <v>223</v>
       </c>
-      <c r="G67" s="0" t="n">
-        <f aca="false">LEN(TRIM(E67))-LEN(SUBSTITUTE(E67," ",""))+1</f>
+      <c r="H67" s="0" t="n">
+        <f aca="false">LEN(TRIM(F67))-LEN(SUBSTITUTE(F67," ",""))+1</f>
         <v>28</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="I67" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2678,26 +2883,29 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <f aca="false">LEN(E68)</f>
+      <c r="E68" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <f aca="false">LEN(F68)</f>
         <v>216</v>
       </c>
-      <c r="G68" s="0" t="n">
-        <f aca="false">LEN(TRIM(E68))-LEN(SUBSTITUTE(E68," ",""))+1</f>
+      <c r="H68" s="0" t="n">
+        <f aca="false">LEN(TRIM(F68))-LEN(SUBSTITUTE(F68," ",""))+1</f>
         <v>25</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="I68" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2706,26 +2914,29 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <f aca="false">LEN(E69)</f>
+      <c r="E69" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <f aca="false">LEN(F69)</f>
         <v>161</v>
       </c>
-      <c r="G69" s="0" t="n">
-        <f aca="false">LEN(TRIM(E69))-LEN(SUBSTITUTE(E69," ",""))+1</f>
+      <c r="H69" s="0" t="n">
+        <f aca="false">LEN(TRIM(F69))-LEN(SUBSTITUTE(F69," ",""))+1</f>
         <v>22</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="I69" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2734,26 +2945,29 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <f aca="false">LEN(E70)</f>
+      <c r="E70" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <f aca="false">LEN(F70)</f>
         <v>181</v>
       </c>
-      <c r="G70" s="0" t="n">
-        <f aca="false">LEN(TRIM(E70))-LEN(SUBSTITUTE(E70," ",""))+1</f>
+      <c r="H70" s="0" t="n">
+        <f aca="false">LEN(TRIM(F70))-LEN(SUBSTITUTE(F70," ",""))+1</f>
         <v>22</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="I70" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2762,26 +2976,29 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <f aca="false">LEN(E71)</f>
+      <c r="E71" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <f aca="false">LEN(F71)</f>
         <v>156</v>
       </c>
-      <c r="G71" s="0" t="n">
-        <f aca="false">LEN(TRIM(E71))-LEN(SUBSTITUTE(E71," ",""))+1</f>
+      <c r="H71" s="0" t="n">
+        <f aca="false">LEN(TRIM(F71))-LEN(SUBSTITUTE(F71," ",""))+1</f>
         <v>22</v>
       </c>
-      <c r="H71" s="0" t="n">
+      <c r="I71" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2790,26 +3007,29 @@
         <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <f aca="false">LEN(E72)</f>
+      <c r="E72" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <f aca="false">LEN(F72)</f>
         <v>160</v>
       </c>
-      <c r="G72" s="0" t="n">
-        <f aca="false">LEN(TRIM(E72))-LEN(SUBSTITUTE(E72," ",""))+1</f>
+      <c r="H72" s="0" t="n">
+        <f aca="false">LEN(TRIM(F72))-LEN(SUBSTITUTE(F72," ",""))+1</f>
         <v>21</v>
       </c>
-      <c r="H72" s="0" t="n">
+      <c r="I72" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2818,26 +3038,29 @@
         <v>72</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <f aca="false">LEN(E73)</f>
+      <c r="E73" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <f aca="false">LEN(F73)</f>
         <v>98</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <f aca="false">LEN(TRIM(E73))-LEN(SUBSTITUTE(E73," ",""))+1</f>
+      <c r="H73" s="0" t="n">
+        <f aca="false">LEN(TRIM(F73))-LEN(SUBSTITUTE(F73," ",""))+1</f>
         <v>17</v>
       </c>
-      <c r="H73" s="0" t="n">
+      <c r="I73" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2846,26 +3069,29 @@
         <v>73</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <f aca="false">LEN(E74)</f>
+      <c r="E74" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <f aca="false">LEN(F74)</f>
         <v>87</v>
       </c>
-      <c r="G74" s="0" t="n">
-        <f aca="false">LEN(TRIM(E74))-LEN(SUBSTITUTE(E74," ",""))+1</f>
+      <c r="H74" s="0" t="n">
+        <f aca="false">LEN(TRIM(F74))-LEN(SUBSTITUTE(F74," ",""))+1</f>
         <v>9</v>
       </c>
-      <c r="H74" s="0" t="n">
+      <c r="I74" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2874,26 +3100,29 @@
         <v>74</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <f aca="false">LEN(E75)</f>
+      <c r="E75" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <f aca="false">LEN(F75)</f>
         <v>231</v>
       </c>
-      <c r="G75" s="0" t="n">
-        <f aca="false">LEN(TRIM(E75))-LEN(SUBSTITUTE(E75," ",""))+1</f>
+      <c r="H75" s="0" t="n">
+        <f aca="false">LEN(TRIM(F75))-LEN(SUBSTITUTE(F75," ",""))+1</f>
         <v>29</v>
       </c>
-      <c r="H75" s="0" t="n">
+      <c r="I75" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2902,26 +3131,29 @@
         <v>75</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <f aca="false">LEN(E76)</f>
+      <c r="E76" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <f aca="false">LEN(F76)</f>
         <v>247</v>
       </c>
-      <c r="G76" s="0" t="n">
-        <f aca="false">LEN(TRIM(E76))-LEN(SUBSTITUTE(E76," ",""))+1</f>
+      <c r="H76" s="0" t="n">
+        <f aca="false">LEN(TRIM(F76))-LEN(SUBSTITUTE(F76," ",""))+1</f>
         <v>31</v>
       </c>
-      <c r="H76" s="0" t="n">
+      <c r="I76" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2930,26 +3162,29 @@
         <v>76</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <f aca="false">LEN(E77)</f>
+      <c r="E77" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <f aca="false">LEN(F77)</f>
         <v>20</v>
       </c>
-      <c r="G77" s="0" t="n">
-        <f aca="false">LEN(TRIM(E77))-LEN(SUBSTITUTE(E77," ",""))+1</f>
+      <c r="H77" s="0" t="n">
+        <f aca="false">LEN(TRIM(F77))-LEN(SUBSTITUTE(F77," ",""))+1</f>
         <v>3</v>
       </c>
-      <c r="H77" s="0" t="n">
+      <c r="I77" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2958,26 +3193,29 @@
         <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <f aca="false">LEN(E78)</f>
+      <c r="E78" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <f aca="false">LEN(F78)</f>
         <v>273</v>
       </c>
-      <c r="G78" s="0" t="n">
-        <f aca="false">LEN(TRIM(E78))-LEN(SUBSTITUTE(E78," ",""))+1</f>
+      <c r="H78" s="0" t="n">
+        <f aca="false">LEN(TRIM(F78))-LEN(SUBSTITUTE(F78," ",""))+1</f>
         <v>34</v>
       </c>
-      <c r="H78" s="0" t="n">
+      <c r="I78" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2986,26 +3224,29 @@
         <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <f aca="false">LEN(E79)</f>
+      <c r="E79" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <f aca="false">LEN(F79)</f>
         <v>215</v>
       </c>
-      <c r="G79" s="0" t="n">
-        <f aca="false">LEN(TRIM(E79))-LEN(SUBSTITUTE(E79," ",""))+1</f>
+      <c r="H79" s="0" t="n">
+        <f aca="false">LEN(TRIM(F79))-LEN(SUBSTITUTE(F79," ",""))+1</f>
         <v>26</v>
       </c>
-      <c r="H79" s="0" t="n">
+      <c r="I79" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3014,26 +3255,29 @@
         <v>79</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F80" s="0" t="n">
-        <f aca="false">LEN(E80)</f>
+      <c r="E80" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <f aca="false">LEN(F80)</f>
         <v>207</v>
       </c>
-      <c r="G80" s="0" t="n">
-        <f aca="false">LEN(TRIM(E80))-LEN(SUBSTITUTE(E80," ",""))+1</f>
+      <c r="H80" s="0" t="n">
+        <f aca="false">LEN(TRIM(F80))-LEN(SUBSTITUTE(F80," ",""))+1</f>
         <v>27</v>
       </c>
-      <c r="H80" s="0" t="n">
+      <c r="I80" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3042,26 +3286,29 @@
         <v>80</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <f aca="false">LEN(E81)</f>
+      <c r="E81" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <f aca="false">LEN(F81)</f>
         <v>173</v>
       </c>
-      <c r="G81" s="0" t="n">
-        <f aca="false">LEN(TRIM(E81))-LEN(SUBSTITUTE(E81," ",""))+1</f>
+      <c r="H81" s="0" t="n">
+        <f aca="false">LEN(TRIM(F81))-LEN(SUBSTITUTE(F81," ",""))+1</f>
         <v>27</v>
       </c>
-      <c r="H81" s="0" t="n">
+      <c r="I81" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3070,31 +3317,34 @@
         <v>81</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <f aca="false">LEN(E82)</f>
+      <c r="E82" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <f aca="false">LEN(F82)</f>
         <v>192</v>
       </c>
-      <c r="G82" s="0" t="n">
-        <f aca="false">LEN(TRIM(E82))-LEN(SUBSTITUTE(E82," ",""))+1</f>
+      <c r="H82" s="0" t="n">
+        <f aca="false">LEN(TRIM(F82))-LEN(SUBSTITUTE(F82," ",""))+1</f>
         <v>28</v>
       </c>
-      <c r="H82" s="0" t="n">
+      <c r="I82" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F105:F1048576 F2:F82">
+  <conditionalFormatting sqref="G105:G1048576 G2:G82">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="&quot;&lt;500&quot;"/>
@@ -3104,7 +3354,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G82">
+  <conditionalFormatting sqref="H2:H82">
     <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>40</formula>
     </cfRule>
@@ -3117,15 +3367,15 @@
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G82">
+  <conditionalFormatting sqref="H1:H82">
     <cfRule type="cellIs" priority="6" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>0</formula>
     </cfRule>
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>LEN(TRIM(G1))=0</formula>
+      <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F82">
+  <conditionalFormatting sqref="G2:G82">
     <cfRule type="cellIs" priority="8" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>500</formula>
     </cfRule>

</xml_diff>

<commit_message>
back to initial version of topics
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/topics.xlsx
+++ b/epitweetr/inst/extdata/topics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="161">
   <si>
     <t>#</t>
   </si>
@@ -527,78 +527,6 @@
   </si>
   <si>
     <t>"e. coli producteurs de shigatoxines" OR "e. coli produtora de toxina shiga" OR "e. coli shiga-toxigênica" OR "e. coli shigatoxigênica" OR "e. coli vero-toxigênica" OR "e. coli verotoxigênica"</t>
-  </si>
-  <si>
-    <t>Haemorrhagic_fever</t>
-  </si>
-  <si>
-    <t>Avian_influenza</t>
-  </si>
-  <si>
-    <t>West_Nile_virus</t>
-  </si>
-  <si>
-    <t>Crimean-Congo_haemorrhagic_fever</t>
-  </si>
-  <si>
-    <t>Lyme_disease</t>
-  </si>
-  <si>
-    <t>Meningococcal_disease</t>
-  </si>
-  <si>
-    <t>Antimicrobial_resistance</t>
-  </si>
-  <si>
-    <t>Creutzfeld-Jakob_disease</t>
-  </si>
-  <si>
-    <t>Haemophilus_influenzae</t>
-  </si>
-  <si>
-    <t>Clostridium_difficile</t>
-  </si>
-  <si>
-    <t>Hepatitis_A</t>
-  </si>
-  <si>
-    <t>Hepatitis_B-C</t>
-  </si>
-  <si>
-    <t>Seasonal_influenza</t>
-  </si>
-  <si>
-    <t>Lassa_fever</t>
-  </si>
-  <si>
-    <t>Legionnaires_disease</t>
-  </si>
-  <si>
-    <t>Pneumococcal_disease</t>
-  </si>
-  <si>
-    <t>Q_fever</t>
-  </si>
-  <si>
-    <t>Rift_Valley_fever</t>
-  </si>
-  <si>
-    <t>Tick-borne_encephalitis</t>
-  </si>
-  <si>
-    <t>Infectious_diseases</t>
-  </si>
-  <si>
-    <t>Healthcare-associated_infections</t>
-  </si>
-  <si>
-    <t>Vectorborne_diseases</t>
-  </si>
-  <si>
-    <t>Foodborne_diseases</t>
-  </si>
-  <si>
-    <t>Waterborne_diseases</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1285,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1440,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -1471,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -1502,7 +1430,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1843,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -1936,7 +1864,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
@@ -1967,7 +1895,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -2091,7 +2019,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
@@ -2246,7 +2174,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
         <v>78</v>
@@ -2308,7 +2236,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
         <v>82</v>
@@ -2339,7 +2267,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>84</v>
@@ -2370,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
         <v>86</v>
@@ -2463,7 +2391,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
         <v>91</v>
@@ -2494,7 +2422,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
         <v>93</v>
@@ -2525,7 +2453,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
         <v>95</v>
@@ -2680,7 +2608,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>105</v>
@@ -2711,7 +2639,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
         <v>107</v>
@@ -2742,7 +2670,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
         <v>109</v>
@@ -2866,7 +2794,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
         <v>117</v>
@@ -2897,7 +2825,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
         <v>117</v>
@@ -3129,7 +3057,7 @@
         <v>133</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G97" si="4">LEN(F66)</f>
+        <f t="shared" ref="G66:G82" si="4">LEN(F66)</f>
         <v>46</v>
       </c>
       <c r="H66">
@@ -3145,7 +3073,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
         <v>134</v>
@@ -3176,7 +3104,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
         <v>134</v>
@@ -3393,7 +3321,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C75" t="s">
         <v>147</v>
@@ -3424,7 +3352,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
         <v>147</v>
@@ -3486,7 +3414,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="C78" t="s">
         <v>152</v>
@@ -3517,7 +3445,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="C79" t="s">
         <v>154</v>
@@ -3548,7 +3476,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="C80" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
typo in topics.xlsx file
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/topics.xlsx
+++ b/epitweetr/inst/extdata/topics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="keywords for tool" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Avian influenza</t>
-  </si>
-  <si>
-    <t>h1n1 OR h5n1 OR h3n2 OR h2n2 OR "avian flu" OR "bird flu" OR "gripe aviar" OR "grippe aviaire" OR 2gripe aviária"</t>
   </si>
   <si>
     <t>Chikungunya</t>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>"e. coli producteurs de shigatoxines" OR "e. coli produtora de toxina shiga" OR "e. coli shiga-toxigênica" OR "e. coli shigatoxigênica" OR "e. coli vero-toxigênica" OR "e. coli verotoxigênica"</t>
+  </si>
+  <si>
+    <t>h1n1 OR h5n1 OR h3n2 OR h2n2 OR "avian flu" OR "bird flu" OR "gripe aviar" OR "grippe aviaire" OR "gripe aviária"</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
         <v>0.05</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1244,19 +1244,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.05</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1275,19 +1275,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E9">
-        <v>0.05</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -1306,19 +1306,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E10">
-        <v>0.05</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -1337,19 +1337,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E11">
-        <v>0.05</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -1368,19 +1368,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E12">
-        <v>0.05</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -1399,10 +1399,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>2.5000000000000001E-2</v>
@@ -1411,7 +1411,7 @@
         <v>0.05</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -1430,19 +1430,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E14">
-        <v>0.05</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -1461,19 +1461,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E15">
-        <v>0.05</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1492,10 +1492,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>2.5000000000000001E-2</v>
@@ -1504,7 +1504,7 @@
         <v>0.05</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -1523,19 +1523,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E17">
-        <v>0.05</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -1554,19 +1554,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E18">
-        <v>0.05</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -1585,19 +1585,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.05</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E19">
-        <v>0.05</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -1616,10 +1616,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>2.5000000000000001E-2</v>
@@ -1628,7 +1628,7 @@
         <v>0.05</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -1647,19 +1647,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E21">
-        <v>0.05</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -1678,19 +1678,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E22">
-        <v>0.05</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -1709,19 +1709,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.05</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E23">
-        <v>0.05</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -1740,19 +1740,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E24">
-        <v>0.05</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -1771,19 +1771,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.05</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E25">
-        <v>0.05</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -1802,19 +1802,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E26">
-        <v>0.05</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -1833,19 +1833,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E27">
-        <v>0.05</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -1864,19 +1864,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.05</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E28">
-        <v>0.05</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -1895,19 +1895,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E29">
+        <v>0.05</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E29">
-        <v>0.05</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -1926,19 +1926,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E30">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E30">
-        <v>0.05</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -1957,19 +1957,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E31">
-        <v>0.05</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -1988,19 +1988,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E32">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E32">
-        <v>0.05</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -2019,19 +2019,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E33">
-        <v>0.05</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -2050,19 +2050,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E34">
+        <v>0.05</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E34">
-        <v>0.05</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G65" si="2">LEN(F34)</f>
@@ -2081,19 +2081,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.05</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E35">
-        <v>0.05</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="G35">
         <f t="shared" si="2"/>
@@ -2112,19 +2112,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.05</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E36">
-        <v>0.05</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G36">
         <f t="shared" si="2"/>
@@ -2143,19 +2143,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E37">
+        <v>0.05</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E37">
-        <v>0.05</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="G37">
         <f t="shared" si="2"/>
@@ -2174,19 +2174,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E38">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E38">
-        <v>0.05</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G38">
         <f t="shared" si="2"/>
@@ -2205,19 +2205,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E39">
+        <v>0.05</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E39">
-        <v>0.05</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G39">
         <f t="shared" si="2"/>
@@ -2236,19 +2236,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E40">
+        <v>0.05</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E40">
-        <v>0.05</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="G40">
         <f t="shared" si="2"/>
@@ -2267,19 +2267,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E41">
+        <v>0.05</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E41">
-        <v>0.05</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G41">
         <f t="shared" si="2"/>
@@ -2298,19 +2298,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E42">
+        <v>0.05</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E42">
-        <v>0.05</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G42">
         <f t="shared" si="2"/>
@@ -2329,19 +2329,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E43">
+        <v>0.05</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E43">
-        <v>0.05</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G43">
         <f t="shared" si="2"/>
@@ -2360,10 +2360,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44">
         <v>2.5000000000000001E-2</v>
@@ -2372,7 +2372,7 @@
         <v>0.05</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G44">
         <f t="shared" si="2"/>
@@ -2391,19 +2391,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E45">
+        <v>0.05</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E45">
-        <v>0.05</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
@@ -2422,19 +2422,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E46">
+        <v>0.05</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E46">
-        <v>0.05</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
@@ -2453,19 +2453,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.05</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C47" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E47">
-        <v>0.05</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="G47">
         <f t="shared" si="2"/>
@@ -2484,19 +2484,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.05</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E48">
-        <v>0.05</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="G48">
         <f t="shared" si="2"/>
@@ -2515,19 +2515,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E49">
+        <v>0.05</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E49">
-        <v>0.05</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
@@ -2546,19 +2546,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E50">
+        <v>0.05</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C50" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E50">
-        <v>0.05</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
@@ -2577,19 +2577,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E51">
+        <v>0.05</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E51">
-        <v>0.05</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
@@ -2608,19 +2608,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E52">
+        <v>0.05</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C52" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E52">
-        <v>0.05</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
@@ -2639,19 +2639,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E53">
+        <v>0.05</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C53" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E53">
-        <v>0.05</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
@@ -2670,19 +2670,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E54">
+        <v>0.05</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C54" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E54">
-        <v>0.05</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
@@ -2701,19 +2701,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E55">
+        <v>0.05</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C55" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E55">
-        <v>0.05</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
@@ -2732,19 +2732,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.05</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E56">
-        <v>0.05</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="G56">
         <f t="shared" si="2"/>
@@ -2763,19 +2763,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E57">
+        <v>0.05</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C57" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E57">
-        <v>0.05</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
@@ -2794,19 +2794,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E58">
+        <v>0.05</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C58" t="s">
-        <v>117</v>
-      </c>
-      <c r="D58">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E58">
-        <v>0.05</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
@@ -2825,10 +2825,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D59">
         <v>2.5000000000000001E-2</v>
@@ -2837,7 +2837,7 @@
         <v>0.05</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
@@ -2856,19 +2856,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.05</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C60" t="s">
-        <v>120</v>
-      </c>
-      <c r="D60">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E60">
-        <v>0.05</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
@@ -2887,19 +2887,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.05</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C61" t="s">
-        <v>122</v>
-      </c>
-      <c r="D61">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E61">
-        <v>0.05</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
@@ -2918,19 +2918,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E62">
+        <v>0.05</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C62" t="s">
-        <v>124</v>
-      </c>
-      <c r="D62">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E62">
-        <v>0.05</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="G62">
         <f t="shared" si="2"/>
@@ -2949,19 +2949,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E63">
+        <v>0.05</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C63" t="s">
-        <v>126</v>
-      </c>
-      <c r="D63">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E63">
-        <v>0.05</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="G63">
         <f t="shared" si="2"/>
@@ -2980,19 +2980,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E64">
+        <v>0.05</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E64">
-        <v>0.05</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="G64">
         <f t="shared" si="2"/>
@@ -3011,19 +3011,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E65">
+        <v>0.05</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C65" t="s">
-        <v>130</v>
-      </c>
-      <c r="D65">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E65">
-        <v>0.05</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="G65">
         <f t="shared" si="2"/>
@@ -3042,19 +3042,19 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E66">
+        <v>0.05</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C66" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E66">
-        <v>0.05</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="G66">
         <f t="shared" ref="G66:G82" si="4">LEN(F66)</f>
@@ -3073,19 +3073,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E67">
+        <v>0.05</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C67" t="s">
-        <v>134</v>
-      </c>
-      <c r="D67">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E67">
-        <v>0.05</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G67">
         <f t="shared" si="4"/>
@@ -3104,10 +3104,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D68">
         <v>2.5000000000000001E-2</v>
@@ -3116,7 +3116,7 @@
         <v>0.05</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G68">
         <f t="shared" si="4"/>
@@ -3135,19 +3135,19 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
+        <v>136</v>
+      </c>
+      <c r="D69">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E69">
+        <v>0.05</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C69" t="s">
-        <v>137</v>
-      </c>
-      <c r="D69">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E69">
-        <v>0.05</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G69">
         <f t="shared" si="4"/>
@@ -3166,10 +3166,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D70">
         <v>2.5000000000000001E-2</v>
@@ -3178,7 +3178,7 @@
         <v>0.05</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G70">
         <f t="shared" si="4"/>
@@ -3197,19 +3197,19 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E71">
+        <v>0.05</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="C71" t="s">
-        <v>140</v>
-      </c>
-      <c r="D71">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E71">
-        <v>0.05</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="G71">
         <f t="shared" si="4"/>
@@ -3228,19 +3228,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" t="s">
+        <v>141</v>
+      </c>
+      <c r="D72">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.05</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C72" t="s">
-        <v>142</v>
-      </c>
-      <c r="D72">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E72">
-        <v>0.05</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G72">
         <f t="shared" si="4"/>
@@ -3259,19 +3259,19 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E73">
+        <v>0.05</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C73" t="s">
-        <v>144</v>
-      </c>
-      <c r="D73">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E73">
-        <v>0.05</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G73">
         <f t="shared" si="4"/>
@@ -3290,10 +3290,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D74">
         <v>2.5000000000000001E-2</v>
@@ -3302,7 +3302,7 @@
         <v>0.05</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G74">
         <f t="shared" si="4"/>
@@ -3321,19 +3321,19 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E75">
+        <v>0.05</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C75" t="s">
-        <v>147</v>
-      </c>
-      <c r="D75">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E75">
-        <v>0.05</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="G75">
         <f t="shared" si="4"/>
@@ -3352,10 +3352,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D76">
         <v>2.5000000000000001E-2</v>
@@ -3364,7 +3364,7 @@
         <v>0.05</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G76">
         <f t="shared" si="4"/>
@@ -3383,19 +3383,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" t="s">
+        <v>149</v>
+      </c>
+      <c r="D77">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.05</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C77" t="s">
-        <v>150</v>
-      </c>
-      <c r="D77">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E77">
-        <v>0.05</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
@@ -3414,19 +3414,19 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E78">
+        <v>0.05</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C78" t="s">
-        <v>152</v>
-      </c>
-      <c r="D78">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E78">
-        <v>0.05</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
@@ -3445,19 +3445,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" t="s">
+        <v>153</v>
+      </c>
+      <c r="D79">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E79">
+        <v>0.05</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C79" t="s">
-        <v>154</v>
-      </c>
-      <c r="D79">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E79">
-        <v>0.05</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
@@ -3476,19 +3476,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E80">
+        <v>0.05</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C80" t="s">
-        <v>156</v>
-      </c>
-      <c r="D80">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E80">
-        <v>0.05</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="G80">
         <f t="shared" si="4"/>
@@ -3507,19 +3507,19 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E81">
+        <v>0.05</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C81" t="s">
-        <v>158</v>
-      </c>
-      <c r="D81">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E81">
-        <v>0.05</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="G81">
         <f t="shared" si="4"/>
@@ -3538,10 +3538,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D82">
         <v>2.5000000000000001E-2</v>
@@ -3550,7 +3550,7 @@
         <v>0.05</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G82">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Typos and updated users/topics files
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/topics.xlsx
+++ b/epitweetr/inst/extdata/topics.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\epitweetr_github\epitweetr\epitweetr\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lespinosa\github_repos\epitweetr\epitweetr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC23A57-C53D-4AA2-8B2A-68CAD9D83CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10830" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keywords for tool" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="168">
   <si>
     <t>#</t>
   </si>
@@ -560,11 +573,17 @@
   <si>
     <t>(coronavirus OR "novel coronavirus" OR covid-19 OR sars-covid-2 OR "nouveau coronavirus " OR covid19) AND (cluster OR épidémie OR école OR université OR hôpital OR variants)</t>
   </si>
+  <si>
+    <t>Monkeypox</t>
+  </si>
+  <si>
+    <t>monkeypox OR "viruela del mono" OR "viruela del simio" OR "variole du singe" OR "variola des macacos"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -647,6 +666,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1046,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3703,8 +3728,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="14">
+        <v>86</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E87" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G87" s="12">
+        <f t="shared" ref="G87" si="6">LEN(F87)</f>
+        <v>101</v>
+      </c>
+      <c r="H87" s="12">
+        <f t="shared" ref="H87" si="7">LEN(TRIM(F87))-LEN(SUBSTITUTE(F87," ",""))+1</f>
+        <v>17</v>
+      </c>
+      <c r="I87" s="12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G109:G1048576 G2:G86">
+  <conditionalFormatting sqref="G108:G1048576 G2:G87">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="&quot;&lt;500&quot;"/>
@@ -3714,7 +3770,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H86">
+  <conditionalFormatting sqref="H2:H87">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>40</formula>
     </cfRule>
@@ -3727,7 +3783,7 @@
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H86">
+  <conditionalFormatting sqref="H1:H87">
     <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3735,7 +3791,7 @@
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G86">
+  <conditionalFormatting sqref="G2:G87">
     <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThan">
       <formula>500</formula>
     </cfRule>

</xml_diff>